<commit_message>
submitted to journal of hydrology
yay
</commit_message>
<xml_diff>
--- a/Data/Q/Cross_Section_Surveys/LBJ_cross_section.xlsx
+++ b/Data/Q/Cross_Section_Surveys/LBJ_cross_section.xlsx
@@ -505,11 +505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="406061520"/>
-        <c:axId val="406061912"/>
+        <c:axId val="508059408"/>
+        <c:axId val="508055880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="406061520"/>
+        <c:axId val="508059408"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="16"/>
@@ -546,12 +546,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="406061912"/>
+        <c:crossAx val="508055880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="406061912"/>
+        <c:axId val="508055880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,19 +574,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="406061520"/>
+        <c:crossAx val="508059408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -833,11 +835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="406062696"/>
-        <c:axId val="406063088"/>
+        <c:axId val="508053136"/>
+        <c:axId val="508054312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="406062696"/>
+        <c:axId val="508053136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-1"/>
@@ -895,12 +897,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406063088"/>
+        <c:crossAx val="508054312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="406063088"/>
+        <c:axId val="508054312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406062696"/>
+        <c:crossAx val="508053136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1276,11 +1278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="681743568"/>
-        <c:axId val="622343736"/>
+        <c:axId val="508057840"/>
+        <c:axId val="508059800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="681743568"/>
+        <c:axId val="508057840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,13 +1325,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="622343736"/>
+        <c:crossAx val="508059800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="622343736"/>
+        <c:axId val="508059800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="681743568"/>
+        <c:crossAx val="508057840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3472,7 +3474,7 @@
   <dimension ref="A2:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F3" sqref="F3:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3608,7 +3610,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="12">
-        <f t="shared" ref="I6:I26" si="0">H6+MAX($G$6:$G$26)</f>
+        <f>H6+MAX($G$6:$G$26)</f>
         <v>1.46685</v>
       </c>
       <c r="J6">
@@ -3641,19 +3643,19 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="14">
-        <f t="shared" ref="F7:F24" si="1">B7*12*0.0254</f>
+        <f t="shared" ref="F7:F24" si="0">B7*12*0.0254</f>
         <v>0</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" ref="G7:G24" si="2">((C7*12)+D7)*0.0254</f>
+        <f t="shared" ref="G7:G24" si="1">((C7*12)+D7)*0.0254</f>
         <v>1.4223999999999999</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" ref="H7:H24" si="3">-G7</f>
+        <f t="shared" ref="H7:H24" si="2">-G7</f>
         <v>-1.4223999999999999</v>
       </c>
       <c r="I7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I6:I26" si="3">H7+MAX($G$6:$G$26)</f>
         <v>4.4450000000000101E-2</v>
       </c>
       <c r="J7" s="12">
@@ -3695,19 +3697,19 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.30479999999999996</v>
+      </c>
+      <c r="G8" s="9">
         <f t="shared" si="1"/>
-        <v>0.30479999999999996</v>
-      </c>
-      <c r="G8" s="9">
+        <v>1.4604999999999999</v>
+      </c>
+      <c r="H8" s="9">
         <f t="shared" si="2"/>
-        <v>1.4604999999999999</v>
-      </c>
-      <c r="H8" s="9">
+        <v>-1.4604999999999999</v>
+      </c>
+      <c r="I8" s="12">
         <f t="shared" si="3"/>
-        <v>-1.4604999999999999</v>
-      </c>
-      <c r="I8" s="12">
-        <f t="shared" si="0"/>
         <v>6.3500000000000778E-3</v>
       </c>
       <c r="J8" s="12">
@@ -3748,19 +3750,19 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.60959999999999992</v>
+      </c>
+      <c r="G9" s="9">
         <f t="shared" si="1"/>
-        <v>0.60959999999999992</v>
-      </c>
-      <c r="G9" s="9">
+        <v>1.46685</v>
+      </c>
+      <c r="H9" s="9">
         <f t="shared" si="2"/>
-        <v>1.46685</v>
-      </c>
-      <c r="H9" s="9">
+        <v>-1.46685</v>
+      </c>
+      <c r="I9" s="12">
         <f t="shared" si="3"/>
-        <v>-1.46685</v>
-      </c>
-      <c r="I9" s="12">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="12">
@@ -3801,19 +3803,19 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="G10" s="9">
         <f t="shared" si="1"/>
-        <v>0.91439999999999999</v>
-      </c>
-      <c r="G10" s="9">
+        <v>1.4541499999999998</v>
+      </c>
+      <c r="H10" s="9">
         <f t="shared" si="2"/>
-        <v>1.4541499999999998</v>
-      </c>
-      <c r="H10" s="9">
+        <v>-1.4541499999999998</v>
+      </c>
+      <c r="I10" s="12">
         <f t="shared" si="3"/>
-        <v>-1.4541499999999998</v>
-      </c>
-      <c r="I10" s="12">
-        <f t="shared" si="0"/>
         <v>1.2700000000000156E-2</v>
       </c>
       <c r="J10" s="12">
@@ -3854,19 +3856,19 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2191999999999998</v>
+      </c>
+      <c r="G11" s="9">
         <f t="shared" si="1"/>
-        <v>1.2191999999999998</v>
-      </c>
-      <c r="G11" s="9">
+        <v>1.46685</v>
+      </c>
+      <c r="H11" s="9">
         <f t="shared" si="2"/>
-        <v>1.46685</v>
-      </c>
-      <c r="H11" s="9">
+        <v>-1.46685</v>
+      </c>
+      <c r="I11" s="12">
         <f t="shared" si="3"/>
-        <v>-1.46685</v>
-      </c>
-      <c r="I11" s="12">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="12">
@@ -3907,19 +3909,19 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="9">
+        <f t="shared" si="0"/>
+        <v>1.524</v>
+      </c>
+      <c r="G12" s="9">
         <f t="shared" si="1"/>
-        <v>1.524</v>
-      </c>
-      <c r="G12" s="9">
+        <v>1.46685</v>
+      </c>
+      <c r="H12" s="9">
         <f t="shared" si="2"/>
-        <v>1.46685</v>
-      </c>
-      <c r="H12" s="9">
+        <v>-1.46685</v>
+      </c>
+      <c r="I12" s="12">
         <f t="shared" si="3"/>
-        <v>-1.46685</v>
-      </c>
-      <c r="I12" s="12">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="12">
@@ -3960,19 +3962,19 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8288</v>
+      </c>
+      <c r="G13" s="9">
         <f t="shared" si="1"/>
-        <v>1.8288</v>
-      </c>
-      <c r="G13" s="9">
+        <v>1.4541499999999998</v>
+      </c>
+      <c r="H13" s="9">
         <f t="shared" si="2"/>
-        <v>1.4541499999999998</v>
-      </c>
-      <c r="H13" s="9">
+        <v>-1.4541499999999998</v>
+      </c>
+      <c r="I13" s="12">
         <f t="shared" si="3"/>
-        <v>-1.4541499999999998</v>
-      </c>
-      <c r="I13" s="12">
-        <f t="shared" si="0"/>
         <v>1.2700000000000156E-2</v>
       </c>
       <c r="J13" s="12">
@@ -4013,19 +4015,19 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="9">
+        <f t="shared" si="0"/>
+        <v>2.1335999999999999</v>
+      </c>
+      <c r="G14" s="9">
         <f t="shared" si="1"/>
-        <v>2.1335999999999999</v>
-      </c>
-      <c r="G14" s="9">
+        <v>1.42875</v>
+      </c>
+      <c r="H14" s="9">
         <f t="shared" si="2"/>
-        <v>1.42875</v>
-      </c>
-      <c r="H14" s="9">
+        <v>-1.42875</v>
+      </c>
+      <c r="I14" s="12">
         <f t="shared" si="3"/>
-        <v>-1.42875</v>
-      </c>
-      <c r="I14" s="12">
-        <f t="shared" si="0"/>
         <v>3.8100000000000023E-2</v>
       </c>
       <c r="J14" s="12">
@@ -4066,19 +4068,19 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="9">
+        <f t="shared" si="0"/>
+        <v>2.4383999999999997</v>
+      </c>
+      <c r="G15" s="9">
         <f t="shared" si="1"/>
-        <v>2.4383999999999997</v>
-      </c>
-      <c r="G15" s="9">
+        <v>1.4223999999999999</v>
+      </c>
+      <c r="H15" s="9">
         <f t="shared" si="2"/>
-        <v>1.4223999999999999</v>
-      </c>
-      <c r="H15" s="9">
+        <v>-1.4223999999999999</v>
+      </c>
+      <c r="I15" s="12">
         <f t="shared" si="3"/>
-        <v>-1.4223999999999999</v>
-      </c>
-      <c r="I15" s="12">
-        <f t="shared" si="0"/>
         <v>4.4450000000000101E-2</v>
       </c>
       <c r="J15" s="12">
@@ -4119,19 +4121,19 @@
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7431999999999999</v>
+      </c>
+      <c r="G16" s="9">
         <f t="shared" si="1"/>
-        <v>2.7431999999999999</v>
-      </c>
-      <c r="G16" s="9">
+        <v>1.3652499999999999</v>
+      </c>
+      <c r="H16" s="9">
         <f t="shared" si="2"/>
-        <v>1.3652499999999999</v>
-      </c>
-      <c r="H16" s="9">
+        <v>-1.3652499999999999</v>
+      </c>
+      <c r="I16" s="12">
         <f t="shared" si="3"/>
-        <v>-1.3652499999999999</v>
-      </c>
-      <c r="I16" s="12">
-        <f t="shared" si="0"/>
         <v>0.10160000000000013</v>
       </c>
       <c r="J16" s="12">
@@ -4172,19 +4174,19 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="9">
+        <f t="shared" si="0"/>
+        <v>3.048</v>
+      </c>
+      <c r="G17" s="9">
         <f t="shared" si="1"/>
-        <v>3.048</v>
-      </c>
-      <c r="G17" s="9">
+        <v>1.3715999999999999</v>
+      </c>
+      <c r="H17" s="9">
         <f t="shared" si="2"/>
-        <v>1.3715999999999999</v>
-      </c>
-      <c r="H17" s="9">
+        <v>-1.3715999999999999</v>
+      </c>
+      <c r="I17" s="12">
         <f t="shared" si="3"/>
-        <v>-1.3715999999999999</v>
-      </c>
-      <c r="I17" s="12">
-        <f t="shared" si="0"/>
         <v>9.5250000000000057E-2</v>
       </c>
       <c r="J17" s="12">
@@ -4225,19 +4227,19 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="9">
+        <f t="shared" si="0"/>
+        <v>3.3527999999999998</v>
+      </c>
+      <c r="G18" s="9">
         <f t="shared" si="1"/>
-        <v>3.3527999999999998</v>
-      </c>
-      <c r="G18" s="9">
+        <v>1.397</v>
+      </c>
+      <c r="H18" s="9">
         <f t="shared" si="2"/>
-        <v>1.397</v>
-      </c>
-      <c r="H18" s="9">
+        <v>-1.397</v>
+      </c>
+      <c r="I18" s="12">
         <f t="shared" si="3"/>
-        <v>-1.397</v>
-      </c>
-      <c r="I18" s="12">
-        <f t="shared" si="0"/>
         <v>6.9849999999999968E-2</v>
       </c>
       <c r="J18" s="12">
@@ -4278,19 +4280,19 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6576</v>
+      </c>
+      <c r="G19" s="9">
         <f t="shared" si="1"/>
-        <v>3.6576</v>
-      </c>
-      <c r="G19" s="9">
+        <v>1.4033499999999999</v>
+      </c>
+      <c r="H19" s="9">
         <f t="shared" si="2"/>
-        <v>1.4033499999999999</v>
-      </c>
-      <c r="H19" s="9">
+        <v>-1.4033499999999999</v>
+      </c>
+      <c r="I19" s="12">
         <f t="shared" si="3"/>
-        <v>-1.4033499999999999</v>
-      </c>
-      <c r="I19" s="12">
-        <f t="shared" si="0"/>
         <v>6.3500000000000112E-2</v>
       </c>
       <c r="J19" s="12">
@@ -4331,19 +4333,19 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="9">
+        <f t="shared" si="0"/>
+        <v>3.9623999999999997</v>
+      </c>
+      <c r="G20" s="9">
         <f t="shared" si="1"/>
-        <v>3.9623999999999997</v>
-      </c>
-      <c r="G20" s="9">
+        <v>1.4097</v>
+      </c>
+      <c r="H20" s="9">
         <f t="shared" si="2"/>
-        <v>1.4097</v>
-      </c>
-      <c r="H20" s="9">
+        <v>-1.4097</v>
+      </c>
+      <c r="I20" s="12">
         <f t="shared" si="3"/>
-        <v>-1.4097</v>
-      </c>
-      <c r="I20" s="12">
-        <f t="shared" si="0"/>
         <v>5.7150000000000034E-2</v>
       </c>
       <c r="J20" s="12">
@@ -4384,19 +4386,19 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="9">
+        <f t="shared" si="0"/>
+        <v>4.2671999999999999</v>
+      </c>
+      <c r="G21" s="9">
         <f t="shared" si="1"/>
-        <v>4.2671999999999999</v>
-      </c>
-      <c r="G21" s="9">
+        <v>1.3461999999999998</v>
+      </c>
+      <c r="H21" s="9">
         <f t="shared" si="2"/>
-        <v>1.3461999999999998</v>
-      </c>
-      <c r="H21" s="9">
+        <v>-1.3461999999999998</v>
+      </c>
+      <c r="I21" s="12">
         <f t="shared" si="3"/>
-        <v>-1.3461999999999998</v>
-      </c>
-      <c r="I21" s="12">
-        <f t="shared" si="0"/>
         <v>0.12065000000000015</v>
       </c>
       <c r="J21" s="12">
@@ -4437,19 +4439,19 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5720000000000001</v>
+      </c>
+      <c r="G22" s="9">
         <f t="shared" si="1"/>
-        <v>4.5720000000000001</v>
-      </c>
-      <c r="G22" s="9">
+        <v>1.3334999999999999</v>
+      </c>
+      <c r="H22" s="9">
         <f t="shared" si="2"/>
-        <v>1.3334999999999999</v>
-      </c>
-      <c r="H22" s="9">
+        <v>-1.3334999999999999</v>
+      </c>
+      <c r="I22" s="12">
         <f t="shared" si="3"/>
-        <v>-1.3334999999999999</v>
-      </c>
-      <c r="I22" s="12">
-        <f t="shared" si="0"/>
         <v>0.13335000000000008</v>
       </c>
       <c r="J22" s="12">
@@ -4492,19 +4494,19 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="9">
+        <f t="shared" si="0"/>
+        <v>4.7244000000000002</v>
+      </c>
+      <c r="G23" s="9">
         <f t="shared" si="1"/>
-        <v>4.7244000000000002</v>
-      </c>
-      <c r="G23" s="9">
+        <v>1.3208</v>
+      </c>
+      <c r="H23" s="9">
         <f t="shared" si="2"/>
-        <v>1.3208</v>
-      </c>
-      <c r="H23" s="9">
+        <v>-1.3208</v>
+      </c>
+      <c r="I23" s="12">
         <f t="shared" si="3"/>
-        <v>-1.3208</v>
-      </c>
-      <c r="I23" s="12">
-        <f t="shared" si="0"/>
         <v>0.14605000000000001</v>
       </c>
       <c r="J23" s="12">
@@ -4545,19 +4547,19 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="9">
+        <f t="shared" si="0"/>
+        <v>4.8767999999999994</v>
+      </c>
+      <c r="G24" s="9">
         <f t="shared" si="1"/>
-        <v>4.8767999999999994</v>
-      </c>
-      <c r="G24" s="9">
+        <v>1.3144499999999999</v>
+      </c>
+      <c r="H24" s="9">
         <f t="shared" si="2"/>
-        <v>1.3144499999999999</v>
-      </c>
-      <c r="H24" s="9">
+        <v>-1.3144499999999999</v>
+      </c>
+      <c r="I24" s="12">
         <f t="shared" si="3"/>
-        <v>-1.3144499999999999</v>
-      </c>
-      <c r="I24" s="12">
-        <f t="shared" si="0"/>
         <v>0.15240000000000009</v>
       </c>
       <c r="J24" s="12">
@@ -4612,7 +4614,7 @@
         <v>-1.3081</v>
       </c>
       <c r="I25" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.15874999999999995</v>
       </c>
       <c r="J25" s="12">
@@ -4664,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.46685</v>
       </c>
       <c r="J26" s="12">

</xml_diff>